<commit_message>
Signed-off-by: Sebastijonas Valaitis <d.dizya@gmail.com>
</commit_message>
<xml_diff>
--- a/sn2_methylchloride_f_attack/Rezultatai.xlsx
+++ b/sn2_methylchloride_f_attack/Rezultatai.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>gas env</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>CH3Cl</t>
+  </si>
+  <si>
+    <t>SUM</t>
   </si>
   <si>
     <t>F~CH3Cl (pre-RC)</t>
@@ -1050,7 +1053,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1094,9 +1097,6 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1245,6 +1245,871 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000_ </c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-599.757922707703</c:v>
+                </c:pt>
+                <c:pt idx="1" c:formatCode="General">
+                  <c:v>-600.08635</c:v>
+                </c:pt>
+                <c:pt idx="2" c:formatCode="General">
+                  <c:v>-599.781799462202</c:v>
+                </c:pt>
+                <c:pt idx="3" c:formatCode="General">
+                  <c:v>-600.08635797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-599.813439820778</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="0"/>
+        <c:smooth val="0"/>
+        <c:axId val="998775553"/>
+        <c:axId val="284262208"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="998775553"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-GB" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="284262208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="284262208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90200"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000_ " sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-GB" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="998775553"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-GB" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-GB"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="10028">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst/>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="90200"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>415925</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>41275</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="10693400" y="1746250"/>
+        <a:ext cx="4826000" cy="2743200"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1505,10 +2370,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1546,18 +2411,18 @@
         <v>-99.788700031088</v>
       </c>
       <c r="C2" s="6">
-        <f>$C$36*B2</f>
+        <f>$C$38*B2</f>
         <v>-261995.194011916</v>
       </c>
       <c r="D2" s="7">
-        <f>B2*$C$37</f>
+        <f>B2*$C$39</f>
         <v>-62618.3546676518</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" ht="15.75" spans="1:8">
+    <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1565,553 +2430,576 @@
         <v>-499.969222676615</v>
       </c>
       <c r="C3" s="11">
-        <f>$C$36*B3</f>
+        <f>$C$38*B3</f>
         <v>-1312669.00414915</v>
       </c>
       <c r="D3" s="12">
-        <f>B3*$C$37</f>
+        <f>B3*$C$39</f>
         <v>-313735.423937992</v>
       </c>
       <c r="F3" s="8"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" ht="17.25" spans="1:8">
-      <c r="A4" s="13" t="s">
+    <row r="4" ht="15.75" spans="1:2">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16">
+      <c r="B4" s="9">
         <f>B2+B3</f>
         <v>-599.757922707703</v>
       </c>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
+    </row>
+    <row r="5" ht="17.25" spans="1:8">
+      <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="14">
+        <v>-600.08635</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16">
+        <f>B2+B3</f>
+        <v>-599.757922707703</v>
+      </c>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="18">
         <v>-599.781799462202</v>
       </c>
-      <c r="C5" s="6">
-        <f>$C$36*B5</f>
+      <c r="C6" s="6">
+        <f>$C$38*B6</f>
         <v>-1574726.88657093</v>
       </c>
-      <c r="D5" s="7">
-        <f>B5*$C$37</f>
+      <c r="D6" s="7">
+        <f>B6*$C$39</f>
         <v>-376368.7614953</v>
       </c>
-      <c r="E5" s="19"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="16">
-        <f>B7+B8</f>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" ht="15.75" spans="1:7">
+      <c r="A7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="21">
+        <v>-600.08635797</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="16">
+        <f>B9+B10</f>
         <v>-599.813439820778</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="23"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="25">
-        <v>-460.160972294191</v>
-      </c>
-      <c r="C7" s="25">
-        <f>$C$36*B7</f>
-        <v>-1208152.45789723</v>
-      </c>
-      <c r="D7" s="26">
-        <f>B7*$C$37</f>
-        <v>-288755.369679656</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" ht="15.75" spans="1:4">
-      <c r="A8" s="27" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9">
+        <f>SUM(B9:B10)</f>
+        <v>-599.813439820778</v>
+      </c>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B9" s="25">
+        <v>-460.160972294191</v>
+      </c>
+      <c r="C9" s="25">
+        <f>$C$38*B9</f>
+        <v>-1208152.45789723</v>
+      </c>
+      <c r="D9" s="26">
+        <f>B9*$C$39</f>
+        <v>-288755.369679656</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" ht="15.75" spans="1:8">
+      <c r="A10" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="28">
         <v>-139.652467526587</v>
       </c>
-      <c r="C8" s="28">
-        <f>$C$36*B8</f>
+      <c r="C10" s="28">
+        <f>$C$38*B10</f>
         <v>-366657.500423117</v>
       </c>
-      <c r="D8" s="29">
-        <f>B8*$C$37</f>
+      <c r="D10" s="29">
+        <f>B10*$C$39</f>
         <v>-87633.2464404107</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="31">
-        <f>B7+B8-B2-B3</f>
+      <c r="G10" s="23"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="31">
+        <f>B9+B10-B2-B3</f>
         <v>-0.0555171130750409</v>
       </c>
-      <c r="C9" s="31">
-        <f>C7+C8-C2-C3</f>
+      <c r="C11" s="31">
+        <f>C9+C10-C2-C3</f>
         <v>-145.760159282247</v>
       </c>
-      <c r="D9" s="32">
-        <f>D7+D8-D2-D3</f>
+      <c r="D11" s="32">
+        <f>D9+D10-D2-D3</f>
         <v>-34.8375144236488</v>
       </c>
-      <c r="E9" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="5" t="s">
+      <c r="E11" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6">
-        <f>B5-(B3+B2)</f>
+      <c r="F11" s="33"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="6">
+        <f>B6-(B3+B2)</f>
         <v>-0.0238767544990424</v>
       </c>
-      <c r="C10" s="34">
-        <f>$C$36*B10</f>
+      <c r="C12" s="34">
+        <f>$C$38*B12</f>
         <v>-62.688409864069</v>
       </c>
-      <c r="D10" s="35">
-        <f>$C$37*B10</f>
+      <c r="D12" s="35">
+        <f>$C$39*B12</f>
         <v>-14.9828896565212</v>
       </c>
-      <c r="E10" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="37"/>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="27" t="s">
+      <c r="E12" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="28">
-        <f>B5-(B8+B7)</f>
+      <c r="F12" s="36"/>
+    </row>
+    <row r="13" ht="15.75" spans="1:6">
+      <c r="A13" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="28">
+        <f>B6-(B10+B9)</f>
         <v>0.0316403585760554</v>
       </c>
-      <c r="C11" s="38">
-        <f>$C$36*B11</f>
+      <c r="C13" s="37">
+        <f>$C$38*B13</f>
         <v>83.0717494180972</v>
       </c>
-      <c r="D11" s="39">
-        <f>$C$37*B11</f>
+      <c r="D13" s="38">
+        <f>$C$39*B13</f>
         <v>19.8546247672319</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" ht="15.75" spans="5:6">
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="44">
-        <v>78.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="46">
-        <v>-99.929315225336</v>
-      </c>
-      <c r="C14" s="46">
-        <f>$C$36*B14</f>
-        <v>-262364.37915098</v>
-      </c>
-      <c r="D14" s="47">
-        <f>B14*$C$37</f>
-        <v>-62706.5920342308</v>
-      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" ht="15.75" spans="5:6">
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" ht="15.75" spans="1:6">
-      <c r="A15" s="48" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="43">
+        <v>78.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="45">
+        <v>-99.929315225336</v>
+      </c>
+      <c r="C16" s="45">
+        <f>$C$38*B16</f>
+        <v>-262364.37915098</v>
+      </c>
+      <c r="D16" s="46">
+        <f>B16*$C$39</f>
+        <v>-62706.5920342308</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" ht="15.75" spans="1:6">
+      <c r="A17" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B17" s="48">
         <v>-499.973960862446</v>
       </c>
-      <c r="C15" s="49">
-        <f>$C$36*B15</f>
+      <c r="C17" s="48">
+        <f>$C$38*B17</f>
         <v>-1312681.44425425</v>
       </c>
-      <c r="D15" s="50">
-        <f>B15*$C$37</f>
+      <c r="D17" s="49">
+        <f>B17*$C$39</f>
         <v>-313738.39719449</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="53"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="54">
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="53">
         <v>-599.883770337165</v>
       </c>
-      <c r="C17" s="46">
-        <f>$C$36*B17</f>
+      <c r="C19" s="45">
+        <f>$C$38*B19</f>
         <v>-1574994.61106439</v>
       </c>
-      <c r="D17" s="47">
-        <f>B17*$C$37</f>
+      <c r="D19" s="46">
+        <f>B19*$C$39</f>
         <v>-376432.749185411</v>
       </c>
     </row>
-    <row r="18" ht="15.75" spans="1:4">
-      <c r="A18" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="57"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="59">
+    <row r="20" ht="15.75" spans="1:4">
+      <c r="A20" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="58">
         <v>-460.274652550907</v>
       </c>
-      <c r="C19" s="59">
-        <f>$C$36*B19</f>
+      <c r="C21" s="58">
+        <f>$C$38*B21</f>
         <v>-1208450.92536804</v>
       </c>
-      <c r="D19" s="60">
-        <f>B19*$C$37</f>
+      <c r="D21" s="59">
+        <f>B21*$C$39</f>
         <v>-288826.705117752</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" ht="15.75" spans="1:6">
-      <c r="A20" s="61" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="62">
-        <v>-139.657362331308</v>
-      </c>
-      <c r="C20" s="62">
-        <f>$C$36*B20</f>
-        <v>-366670.351731052</v>
-      </c>
-      <c r="D20" s="63">
-        <f>B20*$C$37</f>
-        <v>-87636.3179767465</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="65">
-        <f>B19+B20-B14-B15</f>
-        <v>-0.028738794432968</v>
-      </c>
-      <c r="C21" s="65">
-        <f>C19+C20-C14-C15</f>
-        <v>-75.4536938630044</v>
-      </c>
-      <c r="D21" s="66">
-        <f>D19+D20-D14-D15</f>
-        <v>-18.0338657780085</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="46">
-        <f>B17-(B15+B14)</f>
-        <v>0.0195057506170997</v>
-      </c>
-      <c r="C22" s="67">
-        <f>$C$36*B22</f>
-        <v>51.21234083301</v>
-      </c>
-      <c r="D22" s="68">
-        <f>$C$37*B22</f>
-        <v>12.2400433097114</v>
+    <row r="22" ht="15.75" spans="1:6">
+      <c r="A22" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="61">
+        <v>-139.657362331308</v>
+      </c>
+      <c r="C22" s="61">
+        <f>$C$38*B22</f>
+        <v>-366670.351731052</v>
+      </c>
+      <c r="D22" s="62">
+        <f>B22*$C$39</f>
+        <v>-87636.3179767465</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" ht="15.75" spans="1:6">
-      <c r="A23" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="62">
-        <f>B17-(B20+B19)</f>
-        <v>0.0482445450500109</v>
-      </c>
-      <c r="C23" s="69">
-        <f>$C$36*B23</f>
-        <v>126.666034695876</v>
-      </c>
-      <c r="D23" s="70">
-        <f>$C$37*B23</f>
-        <v>30.2739090877016</v>
+    <row r="23" spans="1:6">
+      <c r="A23" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="64">
+        <f>B21+B22-B16-B17</f>
+        <v>-0.028738794432968</v>
+      </c>
+      <c r="C23" s="64">
+        <f>C21+C22-C16-C17</f>
+        <v>-75.4536938630044</v>
+      </c>
+      <c r="D23" s="65">
+        <f>D21+D22-D16-D17</f>
+        <v>-18.0338657780085</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" ht="15.75" spans="5:6">
+    <row r="24" spans="1:6">
+      <c r="A24" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="45">
+        <f>B19-(B17+B16)</f>
+        <v>0.0195057506170997</v>
+      </c>
+      <c r="C24" s="66">
+        <f>$C$38*B24</f>
+        <v>51.21234083301</v>
+      </c>
+      <c r="D24" s="67">
+        <f>$C$39*B24</f>
+        <v>12.2400433097114</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="73" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="44">
-        <v>25.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="74" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="75">
-        <v>-99.92545188483</v>
-      </c>
-      <c r="C26" s="75">
-        <f>$C$36*B26</f>
-        <v>-262354.235951949</v>
-      </c>
-      <c r="D26" s="76">
-        <f>B26*$C$37</f>
-        <v>-62704.167751462</v>
-      </c>
+    <row r="25" ht="15.75" spans="1:6">
+      <c r="A25" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="61">
+        <f>B19-(B22+B21)</f>
+        <v>0.0482445450500109</v>
+      </c>
+      <c r="C25" s="68">
+        <f>$C$38*B25</f>
+        <v>126.666034695876</v>
+      </c>
+      <c r="D25" s="69">
+        <f>$C$39*B25</f>
+        <v>30.2739090877016</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" ht="15.75" spans="5:6">
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" ht="15.75" spans="1:6">
-      <c r="A27" s="77" t="s">
+    <row r="27" spans="1:6">
+      <c r="A27" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="43">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="74">
+        <v>-99.92545188483</v>
+      </c>
+      <c r="C28" s="74">
+        <f>$C$38*B28</f>
+        <v>-262354.235951949</v>
+      </c>
+      <c r="D28" s="75">
+        <f>B28*$C$39</f>
+        <v>-62704.167751462</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" ht="15.75" spans="1:6">
+      <c r="A29" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="78">
+      <c r="B29" s="77">
         <v>-499.973803845674</v>
       </c>
-      <c r="C27" s="78">
-        <f>$C$36*B27</f>
+      <c r="C29" s="77">
+        <f>$C$38*B29</f>
         <v>-1312681.03200677</v>
       </c>
-      <c r="D27" s="79">
-        <f>B27*$C$37</f>
+      <c r="D29" s="78">
+        <f>B29*$C$39</f>
         <v>-313738.298664978</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="80" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="81"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="82"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="74" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="83">
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="79" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="80"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="81"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="73" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="82">
         <v>-599.880972882533</v>
       </c>
-      <c r="C29" s="75">
-        <f>$C$36*B29</f>
+      <c r="C31" s="74">
+        <f>$C$38*B31</f>
         <v>-1574987.26634832</v>
       </c>
-      <c r="D29" s="76">
-        <f>B29*$C$37</f>
+      <c r="D31" s="75">
+        <f>B31*$C$39</f>
         <v>-376430.993756126</v>
       </c>
     </row>
-    <row r="30" ht="15.75" spans="1:4">
-      <c r="A30" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="85"/>
-      <c r="C30" s="85"/>
-      <c r="D30" s="86"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="88">
+    <row r="32" ht="15.75" spans="1:4">
+      <c r="A32" s="83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="84"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="85"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="87">
         <v>-460.271504848491</v>
       </c>
-      <c r="C31" s="88">
-        <f>$C$36*B31</f>
+      <c r="C33" s="87">
+        <f>$C$38*B33</f>
         <v>-1208442.66107654</v>
       </c>
-      <c r="D31" s="89">
-        <f>B31*$C$37</f>
+      <c r="D33" s="88">
+        <f>B33*$C$39</f>
         <v>-288824.729904665</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-    </row>
-    <row r="32" ht="15.75" spans="1:6">
-      <c r="A32" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="78">
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" ht="15.75" spans="1:6">
+      <c r="A34" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="77">
         <v>-139.657201344675</v>
       </c>
-      <c r="C32" s="78">
-        <f>$C$36*B32</f>
+      <c r="C34" s="77">
+        <f>$C$38*B34</f>
         <v>-366669.929060708</v>
       </c>
-      <c r="D32" s="79">
-        <f>B32*$C$37</f>
+      <c r="D34" s="78">
+        <f>B34*$C$39</f>
         <v>-87636.2169561091</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="90" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="91">
-        <f>B31+B32-B26-B27</f>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="89" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="90">
+        <f>B33+B34-B28-B29</f>
         <v>-0.0294504626619982</v>
       </c>
-      <c r="C33" s="91">
-        <f>C31+C32-C26-C27</f>
+      <c r="C35" s="90">
+        <f>C33+C34-C28-C29</f>
         <v>-77.3221785279457</v>
       </c>
-      <c r="D33" s="92">
-        <f>D31+D32-D26-D27</f>
+      <c r="D35" s="91">
+        <f>D33+D34-D28-D29</f>
         <v>-18.4804443340981</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="75">
-        <f>B29-(B27+B26)</f>
+      <c r="E35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="74">
+        <f>B31-(B29+B28)</f>
         <v>0.0182828479710224</v>
       </c>
-      <c r="C34" s="93">
-        <f>$C$36*B34</f>
+      <c r="C36" s="92">
+        <f>$C$38*B36</f>
         <v>48.0016104004371</v>
       </c>
-      <c r="D34" s="94">
-        <f>$C$37*B34</f>
+      <c r="D36" s="93">
+        <f>$C$39*B36</f>
         <v>11.4726603135182</v>
       </c>
     </row>
-    <row r="35" ht="15.75" spans="1:4">
-      <c r="A35" s="95" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="96">
-        <f>B29-(B32+B31)</f>
+    <row r="37" ht="15.75" spans="1:4">
+      <c r="A37" s="94" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="95">
+        <f>B31-(B34+B33)</f>
         <v>0.0477333106330207</v>
       </c>
-      <c r="C35" s="97">
-        <f>$C$36*B35</f>
+      <c r="C37" s="96">
+        <f>$C$38*B37</f>
         <v>125.323788928338</v>
       </c>
-      <c r="D35" s="98">
-        <f>$C$37*B35</f>
+      <c r="D37" s="97">
+        <f>$C$39*B37</f>
         <v>29.9531046476054</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="8">
+    <row r="38" spans="2:4">
+      <c r="B38" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="8">
         <v>2625.49962</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4">
-      <c r="C37">
+      <c r="D38" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4">
+      <c r="C39">
         <v>627.509474</v>
       </c>
-      <c r="D37" t="s">
-        <v>25</v>
+      <c r="D39" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E35:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>